<commit_message>
First steps at the IbnP PDF creation Funktion
</commit_message>
<xml_diff>
--- a/Vorlagen/Service_Anforderungen.xlsx
+++ b/Vorlagen/Service_Anforderungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgadmin\Documents\Service aufträge\Vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgadmin\source\repos\ServiceTool\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3B5A13-9025-4CF6-945B-A445E1933309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D189B8-85FC-4EA2-A43D-424D39540DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="7980" windowWidth="21840" windowHeight="13020" xr2:uid="{46B8D164-E609-4757-9EC4-6D22EEC365BE}"/>
+    <workbookView xWindow="270" yWindow="45" windowWidth="21600" windowHeight="16935" xr2:uid="{46B8D164-E609-4757-9EC4-6D22EEC365BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Serviceanforderung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Service</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Anreise:</t>
-  </si>
-  <si>
-    <t>-bitte Auswählen-</t>
   </si>
   <si>
     <t>Melden bei:</t>
@@ -321,7 +318,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -330,8 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,13 +351,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -356,21 +368,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,7 +711,7 @@
   <dimension ref="A1:AU165"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:G9"/>
+      <selection activeCell="C30" sqref="C30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,11 +733,11 @@
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -835,9 +832,9 @@
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -886,14 +883,14 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -939,14 +936,14 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1040,14 +1037,14 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1139,16 +1136,16 @@
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1238,15 +1235,15 @@
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="22"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1334,15 +1331,15 @@
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="22"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="27"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1434,17 +1431,17 @@
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="22"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1534,10 +1531,10 @@
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="19"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1585,13 +1582,13 @@
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="9"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1636,13 +1633,13 @@
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="9"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1687,13 +1684,13 @@
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="9"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1738,13 +1735,13 @@
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1990,15 +1987,13 @@
       <c r="AU25" s="1"/>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2043,13 +2038,13 @@
       <c r="AU26" s="1"/>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>20</v>
+      <c r="A27" s="18" t="s">
+        <v>19</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2094,13 +2089,13 @@
       <c r="AU27" s="1"/>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
-        <v>21</v>
+      <c r="A28" s="18" t="s">
+        <v>20</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2145,15 +2140,13 @@
       <c r="AU28" s="1"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>22</v>
+      <c r="A29" s="18" t="s">
+        <v>21</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2198,15 +2191,13 @@
       <c r="AU29" s="1"/>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>23</v>
+      <c r="A30" s="18" t="s">
+        <v>22</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2350,7 +2341,7 @@
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2499,7 +2490,7 @@
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2549,14 +2540,14 @@
       <c r="AU36" s="1"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>26</v>
+      <c r="A37" s="20" t="s">
+        <v>25</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -2600,14 +2591,14 @@
       <c r="AU37" s="1"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>27</v>
+      <c r="A38" s="20" t="s">
+        <v>26</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -2651,14 +2642,14 @@
       <c r="AU38" s="1"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>28</v>
+      <c r="A39" s="20" t="s">
+        <v>27</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2752,12 +2743,12 @@
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
@@ -2903,7 +2894,7 @@
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2953,14 +2944,14 @@
       <c r="AU44" s="1"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -3002,14 +2993,14 @@
       <c r="AU45" s="1"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -3051,14 +3042,14 @@
       <c r="AU46" s="1"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -3100,14 +3091,14 @@
       <c r="AU47" s="1"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -3149,14 +3140,14 @@
       <c r="AU48" s="1"/>
     </row>
     <row r="49" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -3198,14 +3189,14 @@
       <c r="AU49" s="1"/>
     </row>
     <row r="50" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -3247,14 +3238,14 @@
       <c r="AU50" s="1"/>
     </row>
     <row r="51" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3296,14 +3287,14 @@
       <c r="AU51" s="1"/>
     </row>
     <row r="52" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -3345,14 +3336,14 @@
       <c r="AU52" s="1"/>
     </row>
     <row r="53" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -8540,31 +8531,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A45:H53"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B18:C18"/>
@@ -8579,6 +8545,31 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A45:H53"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>